<commit_message>
rearranging repo and sifting through papers that actually have usable data
</commit_message>
<xml_diff>
--- a/data extraction /lit search metadata /pulsepress/pulse_press7jun21.xlsx
+++ b/data extraction /lit search metadata /pulsepress/pulse_press7jun21.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /lit search metadata /pulsepress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07DB3FC3-A080-1442-9570-F1B537C8A324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77268736-9FB9-9345-B71A-9DD187302F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-11640" windowWidth="25060" windowHeight="14400" xr2:uid="{2F64D7F4-80DD-A349-895A-5329DF1C15C9}"/>
+    <workbookView xWindow="29220" yWindow="-8140" windowWidth="24000" windowHeight="14400" xr2:uid="{2F64D7F4-80DD-A349-895A-5329DF1C15C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -695,7 +695,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1034,7 +1034,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>